<commit_message>
Part designs, utility constants made extern, and Motor_constants rethought.
</commit_message>
<xml_diff>
--- a/motor/operating_curves.xlsx
+++ b/motor/operating_curves.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvyen\OneDrive\workspace\projects\micromouse\motor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvyen\source\repos\micromouse-2\motor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38528CA-6C4F-4907-88C2-2EA116622E67}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF6BFAD-937E-4C3B-9AC0-6812C7097C7B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7365" xr2:uid="{017AE540-3D80-4269-993B-421FB18B5236}"/>
   </bookViews>
@@ -2583,7 +2583,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>